<commit_message>
Migration to OpenL 5.15.2
</commit_message>
<xml_diff>
--- a/MAPPING/trunk/org.openl.rules.mapping.dev.test/src/test/resources/org/openl/rules/mapping/validation/condition/ConditionMethodValidationTest.xlsx
+++ b/MAPPING/trunk/org.openl.rules.mapping.dev.test/src/test/resources/org/openl/rules/mapping/validation/condition/ConditionMethodValidationTest.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="24735" windowHeight="11955" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="24735" windowHeight="11955"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
   <si>
     <t>classA</t>
   </si>
@@ -72,9 +72,6 @@
   </si>
   <si>
     <t>b.anInteger</t>
-  </si>
-  <si>
-    <t>org.dozer</t>
   </si>
   <si>
     <t>return null;</t>
@@ -104,8 +101,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -152,7 +149,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -197,10 +194,21 @@
     </border>
     <border>
       <left/>
-      <right/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -208,7 +216,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -235,25 +243,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -291,7 +305,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -325,6 +339,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -359,9 +374,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -534,14 +550,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C7:H17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8:C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="13.5703125" customWidth="1"/>
     <col min="4" max="4" width="34.5703125" customWidth="1"/>
@@ -550,33 +566,30 @@
     <col min="7" max="8" width="17.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="3:8">
+    <row r="7" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C7" s="9" t="s">
         <v>4</v>
       </c>
       <c r="D7" s="9"/>
     </row>
-    <row r="8" spans="3:8">
-      <c r="C8" s="10" t="s">
+    <row r="8" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C8" s="11" t="s">
         <v>5</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="3:8">
-      <c r="C9" s="11"/>
+    <row r="9" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C9" s="12"/>
       <c r="D9" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="3:8">
-      <c r="C10" s="11"/>
-      <c r="D10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="3:8">
+    <row r="10" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C10" s="10"/>
+    </row>
+    <row r="13" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C13" s="7" t="s">
         <v>14</v>
       </c>
@@ -586,7 +599,7 @@
       <c r="G13" s="8"/>
       <c r="H13" s="8"/>
     </row>
-    <row r="14" spans="3:8">
+    <row r="14" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C14" s="2" t="s">
         <v>0</v>
       </c>
@@ -600,13 +613,13 @@
         <v>3</v>
       </c>
       <c r="G14" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H14" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H14" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="15" spans="3:8" ht="60" customHeight="1">
+    </row>
+    <row r="15" spans="3:8" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C15" s="3" t="s">
         <v>7</v>
       </c>
@@ -626,7 +639,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="3:8">
+    <row r="16" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
         <v>17</v>
       </c>
@@ -640,13 +653,13 @@
         <v>18</v>
       </c>
       <c r="G16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H16" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="3:7">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>17</v>
       </c>
@@ -660,14 +673,14 @@
         <v>18</v>
       </c>
       <c r="G17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="C13:H13"/>
     <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="C8:C9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -675,36 +688,36 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C5:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="65.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="3:3">
+    <row r="5" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C5" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C6" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C8" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="3:3">
-      <c r="C6" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="3:3">
-      <c r="C8" s="5" t="s">
+    <row r="9" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C9" s="6" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="3:3">
-      <c r="C9" s="6" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>